<commit_message>
update to version 0.9
</commit_message>
<xml_diff>
--- a/inst/www/example.xlsx
+++ b/inst/www/example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6afc0ed0ab75e78c/Dokumenty/Doktorat/rSalvador FluCalc/mlemur/www/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="246" documentId="13_ncr:1_{B27DCED2-75AA-E34B-8265-6920D90AED71}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{3A2AF7A0-DA1C-814C-A874-CE1C1D750C39}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="11_EC682698F34127494A3045FBDAD4C88AA1A10DB7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{42AABF74-944A-3141-87DA-A2BE88344A9E}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{33FD9413-CA9C-D140-9FEC-10E3A8201139}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Example 1" sheetId="1" r:id="rId1"/>
@@ -18,26 +18,17 @@
     <sheet name="Example 3" sheetId="5" r:id="rId3"/>
     <sheet name="Example 4 - common mistakes" sheetId="6" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="125725"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="64">
   <si>
     <t>&lt;- Empty rows are allowed</t>
   </si>
@@ -90,9 +81,6 @@
     <t>CV</t>
   </si>
   <si>
-    <t>&lt;- Coefficient of variation of the culture size; optional value; will only be checked if MeanCells value is given, otherwise it will be estimated from the colony counts; however, if MeanCells is given and CV is empty, B0 method will not be available</t>
-  </si>
-  <si>
     <t>&lt;- Plating efficiency on selective medium; optional value; if left empty, mlemur will try to calculate it from VolumeTotal, VolumeSelective, and DilutionSelective; if none are given, it will default to 1</t>
   </si>
   <si>
@@ -109,12 +97,6 @@
   </si>
   <si>
     <t>&lt;- Dilution factor on non-selective medium; optional value; checked only if MeanCells is missing</t>
-  </si>
-  <si>
-    <t>&lt;- Colony counts on non-selecive medium; optional value; checked only if MeanCells is missing; at least one should be provided if you want to calculate mean culture size, and at least two if you want to estimate CV</t>
-  </si>
-  <si>
-    <t>&lt;- Relative fitness of mutants to non-mutants; optional value; if not given for each strain, M-K method will not be available</t>
   </si>
   <si>
     <t>^ Unnamed rows will inherit the name from the one above, so you don't have to (but can) name each row containing colony counts on given medium; you must, however, name the first row!</t>
@@ -190,9 +172,6 @@
     </r>
   </si>
   <si>
-    <t>^ If the parametr names column is missing, mlemur assumes that all data you provided are colony counts on selective medium; MeanCells and PlatingEfficiency will be set to 1</t>
-  </si>
-  <si>
     <t>Your experiment data must be in the first sheet of the file!</t>
   </si>
   <si>
@@ -208,12 +187,6 @@
     <t>MeanCells and PlatingEfficiency will be set to 1</t>
   </si>
   <si>
-    <t>MK and B0 will be disabled</t>
-  </si>
-  <si>
-    <t>B0 will be disabled because there is no information about CV</t>
-  </si>
-  <si>
     <t>&lt;- This is a second row with the same name; it will be ignored</t>
   </si>
   <si>
@@ -238,17 +211,68 @@
     <t>This sheet is the 4th one in the file. mlemur only check the 1st sheet.</t>
   </si>
   <si>
-    <t>&lt;- In Strain 2, the amount plated on selective medium exceed the total culture volume</t>
-  </si>
-  <si>
     <t>You can modify this sheet and use it to upload your data after removing the red text</t>
+  </si>
+  <si>
+    <t>&lt;- Coefficient of variation of the culture size; optional value; if empty, it will be estimated from the colony counts; if there are no colony counts, it will default to 0</t>
+  </si>
+  <si>
+    <t>&lt;- Relative fitness of mutants to non-mutants; optional value; if empty, it defaults to 1</t>
+  </si>
+  <si>
+    <t>Lag</t>
+  </si>
+  <si>
+    <t>Residual</t>
+  </si>
+  <si>
+    <t>Inoculum</t>
+  </si>
+  <si>
+    <t>&lt;- Average number of residual mutations on a selective plate; optional value; if empty, it defaults to 0</t>
+  </si>
+  <si>
+    <t>&lt;- Size of inoculum (number of cells); optional value; if empty, it defaults to 0</t>
+  </si>
+  <si>
+    <t>^ If this whole column is missing, mlemur assumes that all data you provided are colony counts on selective medium; MeanCells and PlatingEfficiency will be set to 1, all optional parameters to default value</t>
+  </si>
+  <si>
+    <t>All optional parameters will be set to default values</t>
+  </si>
+  <si>
+    <t>&lt;- In Strain 2, the amount plated on selective medium exceeds the total culture volume</t>
+  </si>
+  <si>
+    <t>&lt;- Phenotypic lag expressed as number of generations; optional value; if empty, it defaults to 0</t>
+  </si>
+  <si>
+    <t>&lt;- Colony counts on non-selective medium; optional value; checked only if MeanCells is missing; at least one should be provided if you want to calculate mean culture size, and at least two if you want to estimate CV</t>
+  </si>
+  <si>
+    <t>&lt;- The death rate (the same for wild-type and mutant cells); optional value; if empty, it defaults to 0</t>
+  </si>
+  <si>
+    <t>Death</t>
+  </si>
+  <si>
+    <t>must be empty if Lag is specified</t>
+  </si>
+  <si>
+    <t>0.9</t>
+  </si>
+  <si>
+    <t>&lt;- Both Lag and Fitness are specified. Currently it is not possible to account for both at the same time, so it will throw an error.</t>
+  </si>
+  <si>
+    <t>must be empty if Fitness is specified</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -277,6 +301,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -298,7 +337,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -323,6 +362,12 @@
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -637,12 +682,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDF71800-625B-2340-BF89-FC8C6B581536}">
-  <dimension ref="A1:Q33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Q38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.6640625" style="4" customWidth="1"/>
     <col min="2" max="5" width="10.83203125" style="4"/>
@@ -665,7 +712,7 @@
         <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
@@ -688,7 +735,7 @@
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -711,7 +758,7 @@
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="1" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
@@ -736,7 +783,7 @@
         <v>0.05</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -750,47 +797,27 @@
       <c r="P4" s="3"/>
       <c r="Q4" s="3"/>
     </row>
-    <row r="5" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
+    <row r="5" spans="1:17" s="9" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
+        <v>48</v>
+      </c>
       <c r="F5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-      <c r="P5" s="3"/>
-      <c r="Q5" s="3"/>
+        <v>56</v>
+      </c>
+      <c r="N5" s="5" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="6" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="3">
-        <v>2000</v>
-      </c>
-      <c r="C6" s="3">
-        <v>2000</v>
-      </c>
-      <c r="D6" s="3">
-        <v>2000</v>
-      </c>
-      <c r="E6" s="3">
-        <v>2000</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
       <c r="F6" s="1" t="s">
-        <v>19</v>
+        <v>47</v>
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
@@ -799,377 +826,445 @@
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
+      <c r="N6" s="6" t="s">
+        <v>60</v>
+      </c>
       <c r="O6" s="3"/>
       <c r="P6" s="3"/>
       <c r="Q6" s="3"/>
     </row>
-    <row r="7" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:17" s="9" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N7" s="6"/>
+    </row>
+    <row r="8" spans="1:17" s="9" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" s="9" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="3">
+        <v>2000</v>
+      </c>
+      <c r="C10" s="3">
+        <v>2000</v>
+      </c>
+      <c r="D10" s="3">
+        <v>2000</v>
+      </c>
+      <c r="E10" s="3">
+        <v>2000</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
+    </row>
+    <row r="11" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B11" s="3">
         <v>100</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C11" s="3">
         <v>100</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D11" s="3">
         <v>100</v>
-      </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
-      <c r="Q7" s="3"/>
-    </row>
-    <row r="8" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="3">
-        <v>1</v>
-      </c>
-      <c r="C8" s="3">
-        <v>1</v>
-      </c>
-      <c r="D8" s="3">
-        <v>1</v>
-      </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
-      <c r="P8" s="3"/>
-      <c r="Q8" s="3"/>
-    </row>
-    <row r="9" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="3">
-        <v>4</v>
-      </c>
-      <c r="C9" s="3">
-        <v>7</v>
-      </c>
-      <c r="D9" s="3">
-        <v>24</v>
-      </c>
-      <c r="E9" s="3">
-        <v>19</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3">
-        <v>1</v>
-      </c>
-      <c r="C10" s="3">
-        <v>1</v>
-      </c>
-      <c r="D10" s="3">
-        <v>7</v>
-      </c>
-      <c r="E10" s="3">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3">
-        <v>1</v>
-      </c>
-      <c r="C11" s="3">
-        <v>0</v>
-      </c>
-      <c r="D11" s="3">
-        <v>6</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="1" t="s">
-        <v>33</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
     </row>
     <row r="12" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="3"/>
+      <c r="A12" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="B12" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D12" s="3">
-        <v>9</v>
-      </c>
-      <c r="E12" s="3">
-        <v>25</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E12" s="3"/>
       <c r="F12" s="1" t="s">
-        <v>1</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
     </row>
     <row r="13" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="3"/>
+      <c r="A13" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="B13" s="3">
         <v>4</v>
       </c>
       <c r="C13" s="3">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D13" s="3">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="E13" s="3">
-        <v>42</v>
+        <v>19</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
       <c r="B14" s="3">
-        <v>2</v>
-      </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="4"/>
+        <v>1</v>
+      </c>
+      <c r="C14" s="3">
+        <v>1</v>
+      </c>
+      <c r="D14" s="3">
+        <v>7</v>
+      </c>
+      <c r="E14" s="3">
+        <v>9</v>
+      </c>
     </row>
     <row r="15" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
       <c r="B15" s="3">
-        <v>7</v>
-      </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
+        <v>1</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0</v>
+      </c>
+      <c r="D15" s="3">
+        <v>6</v>
+      </c>
       <c r="E15" s="3"/>
+      <c r="F15" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="16" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
       <c r="B16" s="3">
-        <v>6</v>
-      </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
+        <v>0</v>
+      </c>
+      <c r="C16" s="3">
+        <v>2</v>
+      </c>
+      <c r="D16" s="3">
+        <v>9</v>
+      </c>
+      <c r="E16" s="3">
+        <v>25</v>
+      </c>
       <c r="F16" s="1" t="s">
-        <v>32</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3">
+        <v>4</v>
+      </c>
+      <c r="C17" s="3">
+        <v>2</v>
+      </c>
+      <c r="D17" s="3">
+        <v>8</v>
+      </c>
+      <c r="E17" s="3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3">
+        <v>2</v>
+      </c>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="4"/>
+    </row>
+    <row r="19" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3">
         <v>7</v>
       </c>
-      <c r="B17" s="3">
-        <v>50</v>
-      </c>
-      <c r="C17" s="3">
-        <v>50</v>
-      </c>
-      <c r="D17" s="3">
-        <v>100</v>
-      </c>
-      <c r="E17" s="3">
-        <v>50</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
-      <c r="N17" s="3"/>
-      <c r="O17" s="3"/>
-      <c r="P17" s="3"/>
-      <c r="Q17" s="3"/>
-    </row>
-    <row r="18" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" s="3">
-        <v>1000000</v>
-      </c>
-      <c r="C18" s="3">
-        <v>1000000</v>
-      </c>
-      <c r="D18" s="3">
-        <v>1000000</v>
-      </c>
-      <c r="E18" s="3">
-        <v>1000000</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
-      <c r="N18" s="3"/>
-      <c r="O18" s="3"/>
-      <c r="P18" s="3"/>
-      <c r="Q18" s="3"/>
-    </row>
-    <row r="19" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" s="3">
-        <v>153</v>
-      </c>
-      <c r="C19" s="3">
-        <v>177</v>
-      </c>
-      <c r="D19" s="3">
-        <v>136</v>
-      </c>
-      <c r="E19" s="3">
-        <v>126</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
     </row>
     <row r="20" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
       <c r="B20" s="3">
+        <v>6</v>
+      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="3">
+        <v>50</v>
+      </c>
+      <c r="C21" s="3">
+        <v>50</v>
+      </c>
+      <c r="D21" s="3">
+        <v>100</v>
+      </c>
+      <c r="E21" s="3">
+        <v>50</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="3"/>
+    </row>
+    <row r="22" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="C22" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="D22" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="E22" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="3"/>
+      <c r="P22" s="3"/>
+      <c r="Q22" s="3"/>
+    </row>
+    <row r="23" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" s="3">
+        <v>153</v>
+      </c>
+      <c r="C23" s="3">
+        <v>177</v>
+      </c>
+      <c r="D23" s="3">
+        <v>136</v>
+      </c>
+      <c r="E23" s="3">
+        <v>126</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3">
         <v>119</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C24" s="3">
         <v>133</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D24" s="3">
         <v>102</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E24" s="3">
         <v>118</v>
       </c>
     </row>
-    <row r="21" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3">
+    <row r="25" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3">
         <v>161</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D25" s="3">
         <v>112</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E25" s="3">
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3">
+    <row r="26" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="3"/>
+      <c r="F26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J26" s="10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3">
         <v>88</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C27" s="3">
         <v>82</v>
       </c>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3">
+      <c r="D27" s="3"/>
+      <c r="E27" s="3">
         <v>92</v>
       </c>
-      <c r="F22" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J22" s="1" t="s">
+    </row>
+    <row r="28" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B28" s="3">
+        <v>107</v>
+      </c>
+      <c r="C28" s="3">
+        <v>122</v>
+      </c>
+      <c r="D28" s="3">
+        <v>82</v>
+      </c>
+      <c r="E28" s="3">
+        <v>103</v>
+      </c>
+      <c r="J28" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="J29" s="6"/>
+    </row>
+    <row r="30" spans="1:17" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3">
-        <v>107</v>
-      </c>
-      <c r="C23" s="3">
-        <v>122</v>
-      </c>
-      <c r="D23" s="3">
-        <v>82</v>
-      </c>
-      <c r="E23" s="3">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J24" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F30" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
+    <row r="31" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F35" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B38" s="7"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB2A5CE3-0FA9-D044-86C1-999696E594C2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
@@ -1197,7 +1292,7 @@
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1209,7 +1304,7 @@
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1221,7 +1316,7 @@
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="1" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1264,12 +1359,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FF07004-162E-2D47-955A-FFA3C37695CC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Q18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.6640625" style="4" customWidth="1"/>
     <col min="2" max="5" width="10.83203125" style="4"/>
@@ -1353,7 +1450,7 @@
         <v>0.95</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1387,9 +1484,7 @@
       <c r="E6" s="3">
         <v>9</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>42</v>
-      </c>
+      <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
@@ -1478,7 +1573,7 @@
         <v>50</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1503,12 +1598,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF8F307A-1A5A-F64B-9A48-7AFDDA122296}">
-  <dimension ref="A1:Q31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:Q33"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.6640625" style="4" customWidth="1"/>
     <col min="2" max="5" width="10.83203125" style="4"/>
@@ -1557,7 +1654,7 @@
         <v>100</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -1616,7 +1713,7 @@
         <v>100</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -1647,7 +1744,7 @@
         <v>1000</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -1690,259 +1787,306 @@
       <c r="Q6" s="3"/>
     </row>
     <row r="7" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="3">
-        <v>4</v>
-      </c>
-      <c r="C7" s="3">
-        <v>7</v>
-      </c>
-      <c r="D7" s="3">
-        <v>1</v>
-      </c>
+      <c r="A7" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
       <c r="E7" s="3">
-        <v>19</v>
-      </c>
-      <c r="F7" s="4"/>
+        <v>1</v>
+      </c>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
     </row>
     <row r="8" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3">
-        <v>1</v>
-      </c>
-      <c r="C8" s="3">
-        <v>1</v>
-      </c>
+      <c r="A8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>44</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
     </row>
     <row r="9" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="3"/>
+      <c r="A9" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="B9" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C9" s="3">
-        <v>0</v>
-      </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
+        <v>7</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1</v>
+      </c>
+      <c r="E9" s="3">
+        <v>19</v>
+      </c>
+      <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
       <c r="B10" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D10" s="3"/>
-      <c r="E10" s="3">
-        <v>25</v>
+      <c r="E10" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
       <c r="B11" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C11" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D11" s="3"/>
-      <c r="E11" s="3">
-        <v>42</v>
-      </c>
+      <c r="E11" s="3"/>
     </row>
     <row r="12" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
       <c r="B12" s="3">
+        <v>0</v>
+      </c>
+      <c r="C12" s="3">
         <v>2</v>
       </c>
-      <c r="C12" s="3"/>
       <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="4"/>
+      <c r="E12" s="3">
+        <v>25</v>
+      </c>
     </row>
     <row r="13" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
       <c r="B13" s="3">
-        <v>7</v>
-      </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E13" s="3"/>
+        <v>4</v>
+      </c>
+      <c r="C13" s="3">
+        <v>2</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3">
+        <v>42</v>
+      </c>
     </row>
     <row r="14" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
       <c r="B14" s="3">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
+      <c r="F14" s="4"/>
     </row>
     <row r="15" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3">
         <v>7</v>
       </c>
-      <c r="B15" s="3">
+      <c r="C15" s="3"/>
+      <c r="D15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3">
+        <v>6</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+    </row>
+    <row r="17" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="3">
         <v>50</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C17" s="3">
         <v>50</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D17" s="3">
         <v>100</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E17" s="3">
         <v>50</v>
       </c>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
-      <c r="N15" s="3"/>
-      <c r="O15" s="3"/>
-      <c r="P15" s="3"/>
-      <c r="Q15" s="3"/>
-    </row>
-    <row r="16" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="3"/>
+    </row>
+    <row r="18" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B18" s="3">
         <v>1000000</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C18" s="3">
         <v>1000000</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D18" s="3">
         <v>1000000</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E18" s="3">
         <v>1000000</v>
       </c>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
-      <c r="N16" s="3"/>
-      <c r="O16" s="3"/>
-      <c r="P16" s="3"/>
-      <c r="Q16" s="3"/>
-    </row>
-    <row r="17" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B17" s="3">
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+      <c r="P18" s="3"/>
+      <c r="Q18" s="3"/>
+    </row>
+    <row r="19" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="3">
         <v>153</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C19" s="3">
         <v>177</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D19" s="3">
         <v>136</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E19" s="3">
         <v>126</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B18" s="3">
+    <row r="20" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="3">
         <v>119</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C20" s="3">
         <v>133</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D20" s="3">
         <v>102</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E20" s="3">
         <v>118</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3">
+    <row r="21" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3">
         <v>161</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D21" s="3">
         <v>112</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E21" s="3">
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3">
+    <row r="22" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3">
         <v>88</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C22" s="3">
         <v>82</v>
       </c>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3">
+      <c r="D22" s="3"/>
+      <c r="E22" s="3">
         <v>92</v>
       </c>
-      <c r="J20" s="1"/>
-    </row>
-    <row r="21" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3">
+      <c r="J22" s="1"/>
+    </row>
+    <row r="23" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3">
         <v>107</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C23" s="3">
         <v>122</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D23" s="3">
         <v>82</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E23" s="3">
         <v>103</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F22" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="J22" s="6"/>
-    </row>
-    <row r="23" spans="1:10" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="2"/>
-    </row>
-    <row r="25" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="2"/>
-    </row>
-    <row r="26" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="2"/>
-    </row>
-    <row r="31" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
+    <row r="24" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F24" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="J24" s="6"/>
+    </row>
+    <row r="25" spans="1:17" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="2"/>
+    </row>
+    <row r="27" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="2"/>
+    </row>
+    <row r="28" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B28" s="2"/>
+    </row>
+    <row r="33" spans="2:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>